<commit_message>
feat: add data analytics
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Kazakhstan_analytics\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FCCD8C-5410-4F4F-BBC9-4D14EA7AAEA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Assignment_4_excel" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Assignment_4_excel"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -28,6 +22,18 @@
     <t>Country</t>
   </si>
   <si>
+    <t xml:space="preserve"> Fertility_Rate_Person_Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Life_Expectancy_Person</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Count_Person_Is_Internet_User_PerCapita</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Growth_Rate_Count_Person</t>
+  </si>
+  <si>
     <t xml:space="preserve"> Count_Person</t>
   </si>
   <si>
@@ -284,24 +290,13 @@
   </si>
   <si>
     <t>90.92</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Fertility_Rate_Person_Female</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Life_Expectancy_Person</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Count_Person_Is_Internet_User_PerCapita</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Growth_Rate_Count_Person</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -344,32 +339,35 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="7">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="49" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -380,10 +378,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -421,71 +419,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -513,7 +511,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -536,11 +534,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -549,13 +547,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -565,7 +563,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -574,7 +572,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -583,7 +581,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -591,10 +589,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -659,62 +657,60 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:G63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.21875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.5546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.88671875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="4" width="5.433571428571429" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="10.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="26.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="21.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="37.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="25.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="12.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>88</v>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>90</v>
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>91</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="1">
         <v>1960</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>4</v>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="D2" s="1">
-        <v>58.370512195121997</v>
+        <v>58.370512195122</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
@@ -726,41 +722,41 @@
         <v>9319283</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1">
         <v>1961</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="D3" s="1">
-        <v>58.503073170731703</v>
+        <v>58.5030731707317</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
       </c>
       <c r="F3" s="1">
-        <v>3.3763004954301699</v>
+        <v>3.37630049543017</v>
       </c>
       <c r="G3" s="1">
         <v>9639302</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1">
         <v>1962</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D4" s="1">
-        <v>58.621756097560997</v>
+        <v>58.621756097561</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
@@ -772,84 +768,84 @@
         <v>9959414</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1">
         <v>1963</v>
       </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>7</v>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="D5" s="1">
-        <v>58.944512195122002</v>
+        <v>58.944512195122</v>
       </c>
       <c r="E5" s="1">
         <v>0</v>
       </c>
       <c r="F5" s="1">
-        <v>3.1467021846367502</v>
+        <v>3.14670218463675</v>
       </c>
       <c r="G5" s="1">
         <v>1027779</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1">
         <v>1964</v>
       </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>8</v>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
       </c>
       <c r="D6" s="1">
-        <v>59.157487804878102</v>
+        <v>59.1574878048781</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
       </c>
       <c r="F6" s="1">
-        <v>3.0013095765307001</v>
+        <v>3.0013095765307</v>
       </c>
       <c r="G6" s="1">
         <v>10590934</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1">
         <v>1965</v>
       </c>
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>9</v>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="D7" s="1">
-        <v>59.461682926829297</v>
+        <v>59.4616829268293</v>
       </c>
       <c r="E7" s="1">
         <v>0</v>
       </c>
       <c r="F7" s="1">
-        <v>2.8548266947074201</v>
+        <v>2.85482669470742</v>
       </c>
       <c r="G7" s="1">
         <v>10897644</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="1">
         <v>1966</v>
       </c>
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>10</v>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="D8" s="1">
         <v>59.6992195121951</v>
@@ -864,15 +860,15 @@
         <v>11197568</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="1">
         <v>1967</v>
       </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>11</v>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="D9" s="1">
         <v>59.8734146341464</v>
@@ -887,84 +883,84 @@
         <v>11491228</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="1">
         <v>1968</v>
       </c>
-      <c r="B10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>12</v>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="D10" s="1">
-        <v>59.998365853658498</v>
+        <v>59.9983658536585</v>
       </c>
       <c r="E10" s="1">
         <v>0</v>
       </c>
       <c r="F10" s="1">
-        <v>2.4636602233543701</v>
+        <v>2.46366022335437</v>
       </c>
       <c r="G10" s="1">
         <v>11777849</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="1">
         <v>1969</v>
       </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>13</v>
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="D11" s="1">
-        <v>60.191170731707302</v>
+        <v>60.1911707317073</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
       </c>
       <c r="F11" s="1">
-        <v>2.2219668730001998</v>
+        <v>2.2219668730002</v>
       </c>
       <c r="G11" s="1">
         <v>12042478</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="1">
         <v>1970</v>
       </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>14</v>
+      <c r="B12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>18</v>
       </c>
       <c r="D12" s="1">
-        <v>60.422975609756101</v>
+        <v>60.4229756097561</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
       </c>
       <c r="F12" s="1">
-        <v>1.8334312253056499</v>
+        <v>1.83343122530565</v>
       </c>
       <c r="G12" s="1">
         <v>12265305</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="1">
         <v>1971</v>
       </c>
-      <c r="B13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>15</v>
+      <c r="B13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="D13" s="1">
         <v>60.6475609756098</v>
@@ -979,18 +975,18 @@
         <v>12444338</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
       <c r="A14" s="1">
         <v>1972</v>
       </c>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>16</v>
+      <c r="B14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="D14" s="1">
-        <v>60.994951219512203</v>
+        <v>60.9949512195122</v>
       </c>
       <c r="E14" s="1">
         <v>0</v>
@@ -1002,18 +998,18 @@
         <v>12611997</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="1">
         <v>1973</v>
       </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>17</v>
+      <c r="B15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="D15" s="1">
-        <v>61.277390243902403</v>
+        <v>61.2773902439024</v>
       </c>
       <c r="E15" s="1">
         <v>0</v>
@@ -1025,61 +1021,61 @@
         <v>12789985</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="1">
         <v>1974</v>
       </c>
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>18</v>
+      <c r="B16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>22</v>
       </c>
       <c r="D16" s="1">
-        <v>61.524975609756098</v>
+        <v>61.5249756097561</v>
       </c>
       <c r="E16" s="1">
         <v>0</v>
       </c>
       <c r="F16" s="1">
-        <v>1.4169058202478999</v>
+        <v>1.4169058202479</v>
       </c>
       <c r="G16" s="1">
         <v>12972497</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
       <c r="A17" s="1">
         <v>1975</v>
       </c>
-      <c r="B17" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>19</v>
+      <c r="B17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="D17" s="1">
-        <v>61.790609756097602</v>
+        <v>61.7906097560976</v>
       </c>
       <c r="E17" s="1">
         <v>0</v>
       </c>
       <c r="F17" s="1">
-        <v>1.4270026527231101</v>
+        <v>1.42700265272311</v>
       </c>
       <c r="G17" s="1">
         <v>13158942</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="1">
         <v>1976</v>
       </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>20</v>
+      <c r="B18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="D18" s="1">
         <v>61.6403414634146</v>
@@ -1088,67 +1084,67 @@
         <v>0</v>
       </c>
       <c r="F18" s="1">
-        <v>1.4128149554317999</v>
+        <v>1.4128149554318</v>
       </c>
       <c r="G18" s="1">
         <v>13346173</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="1">
         <v>1977</v>
       </c>
-      <c r="B19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>21</v>
+      <c r="B19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="D19" s="1">
-        <v>61.853000000000002</v>
+        <v>61.853</v>
       </c>
       <c r="E19" s="1">
         <v>0</v>
       </c>
       <c r="F19" s="1">
-        <v>1.4678600908764501</v>
+        <v>1.46786009087645</v>
       </c>
       <c r="G19" s="1">
         <v>13543521</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
       <c r="A20" s="1">
         <v>1978</v>
       </c>
-      <c r="B20" t="s">
-        <v>3</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>22</v>
+      <c r="B20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="D20" s="1">
-        <v>62.065609756097601</v>
+        <v>62.0656097560976</v>
       </c>
       <c r="E20" s="1">
         <v>0</v>
       </c>
       <c r="F20" s="1">
-        <v>1.5151709533383999</v>
+        <v>1.5151709533384</v>
       </c>
       <c r="G20" s="1">
         <v>13750291</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="1">
         <v>1979</v>
       </c>
-      <c r="B21" t="s">
-        <v>3</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>23</v>
+      <c r="B21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="D21" s="1">
         <v>62.2545853658537</v>
@@ -1157,90 +1153,90 @@
         <v>0</v>
       </c>
       <c r="F21" s="1">
-        <v>1.4978146044212199</v>
+        <v>1.49781460442122</v>
       </c>
       <c r="G21" s="1">
         <v>13957795</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="1">
         <v>1980</v>
       </c>
-      <c r="B22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>24</v>
+      <c r="B22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="D22" s="1">
-        <v>66.624390243902496</v>
+        <v>66.6243902439025</v>
       </c>
       <c r="E22" s="1">
         <v>0</v>
       </c>
       <c r="F22" s="1">
-        <v>1.5280150965452901</v>
+        <v>1.52801509654529</v>
       </c>
       <c r="G22" s="1">
         <v>1417271</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="1">
         <v>1981</v>
       </c>
-      <c r="B23" t="s">
-        <v>3</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>25</v>
+      <c r="B23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="D23" s="1">
-        <v>66.706097560975607</v>
+        <v>66.7060975609756</v>
       </c>
       <c r="E23" s="1">
         <v>0</v>
       </c>
       <c r="F23" s="1">
-        <v>1.5728725076557299</v>
+        <v>1.57287250765573</v>
       </c>
       <c r="G23" s="1">
         <v>14397391</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="1">
         <v>1982</v>
       </c>
-      <c r="B24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>26</v>
+      <c r="B24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="D24" s="1">
-        <v>66.787804878048803</v>
+        <v>66.7878048780488</v>
       </c>
       <c r="E24" s="1">
         <v>0</v>
       </c>
       <c r="F24" s="1">
-        <v>1.6312810564795299</v>
+        <v>1.63128105647953</v>
       </c>
       <c r="G24" s="1">
         <v>14634179</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="1">
         <v>1983</v>
       </c>
-      <c r="B25" t="s">
-        <v>3</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>27</v>
+      <c r="B25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="D25" s="1">
         <v>67.6621951219512</v>
@@ -1255,133 +1251,133 @@
         <v>14885966</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="1">
         <v>1984</v>
       </c>
-      <c r="B26" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>28</v>
+      <c r="B26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="D26" s="1">
-        <v>68.536585365853696</v>
+        <v>68.5365853658537</v>
       </c>
       <c r="E26" s="1">
         <v>0</v>
       </c>
       <c r="F26" s="1">
-        <v>1.7422553484021299</v>
+        <v>1.74225534840213</v>
       </c>
       <c r="G26" s="1">
         <v>1514759</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="1">
         <v>1985</v>
       </c>
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>28</v>
+      <c r="B27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="D27" s="1">
-        <v>68.536585365853696</v>
+        <v>68.5365853658537</v>
       </c>
       <c r="E27" s="1">
         <v>0</v>
       </c>
       <c r="F27" s="1">
-        <v>1.7390302855065101</v>
+        <v>1.73903028550651</v>
       </c>
       <c r="G27" s="1">
         <v>15413315</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="1">
         <v>1986</v>
       </c>
-      <c r="B28" t="s">
-        <v>3</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>29</v>
+      <c r="B28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="D28" s="1">
-        <v>68.913414634146307</v>
+        <v>68.9134146341463</v>
       </c>
       <c r="E28" s="1">
         <v>0</v>
       </c>
       <c r="F28" s="1">
-        <v>1.9784034845985401</v>
+        <v>1.97840348459854</v>
       </c>
       <c r="G28" s="1">
         <v>15721289</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="1">
         <v>1987</v>
       </c>
-      <c r="B29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>30</v>
+      <c r="B29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="D29" s="1">
-        <v>69.290243902439002</v>
+        <v>69.290243902439</v>
       </c>
       <c r="E29" s="1">
         <v>0</v>
       </c>
       <c r="F29" s="1">
-        <v>2.2092587140208599</v>
+        <v>2.20925871402086</v>
       </c>
       <c r="G29" s="1">
         <v>16072478</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
       <c r="A30" s="1">
         <v>1988</v>
       </c>
-      <c r="B30" t="s">
-        <v>3</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>31</v>
+      <c r="B30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="D30" s="1">
-        <v>68.848780487804902</v>
+        <v>68.8487804878049</v>
       </c>
       <c r="E30" s="1">
         <v>0</v>
       </c>
       <c r="F30" s="1">
-        <v>2.2036473090175202</v>
+        <v>2.20364730901752</v>
       </c>
       <c r="G30" s="1">
         <v>1643059</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
       <c r="A31" s="1">
         <v>1989</v>
       </c>
-      <c r="B31" t="s">
-        <v>3</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>32</v>
+      <c r="B31" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="D31" s="1">
-        <v>68.290243902439002</v>
+        <v>68.290243902439</v>
       </c>
       <c r="E31" s="1">
         <v>0</v>
@@ -1393,113 +1389,113 @@
         <v>162495</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
       <c r="A32" s="1">
         <v>1990</v>
       </c>
-      <c r="B32" t="s">
-        <v>3</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>33</v>
+      <c r="B32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="D32" s="1">
-        <v>68.336585365853693</v>
+        <v>68.3365853658537</v>
       </c>
       <c r="E32" s="1">
         <v>0</v>
       </c>
       <c r="F32" s="1">
-        <v>0.60434266304362005</v>
+        <v>0.60434266304362</v>
       </c>
       <c r="G32" s="1">
         <v>16348</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
       <c r="A33" s="1">
         <v>1991</v>
       </c>
-      <c r="B33" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>35</v>
+      <c r="B33" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="D33" s="1">
-        <v>67.599999999999994</v>
+        <v>67.6</v>
       </c>
       <c r="E33" s="1">
         <v>0</v>
       </c>
       <c r="F33" s="1">
-        <v>0.63239182585152598</v>
+        <v>0.632391825851526</v>
       </c>
       <c r="G33" s="1">
         <v>16451711</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
       <c r="A34" s="1">
         <v>1992</v>
       </c>
-      <c r="B34" t="s">
-        <v>34</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>36</v>
+      <c r="B34" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="D34" s="1">
-        <v>67.400000000000006</v>
+        <v>67.4</v>
       </c>
       <c r="E34" s="1">
         <v>0</v>
       </c>
       <c r="F34" s="1">
-        <v>-7.6714450954581501E-2</v>
+        <v>-0.0767144509545815</v>
       </c>
       <c r="G34" s="1">
         <v>16439095</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
       <c r="A35" s="1">
         <v>1993</v>
       </c>
-      <c r="B35" t="s">
-        <v>34</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>37</v>
+      <c r="B35" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="D35" s="1">
-        <v>65.400000000000006</v>
+        <v>65.4</v>
       </c>
       <c r="E35" s="1">
         <v>0</v>
       </c>
       <c r="F35" s="1">
-        <v>-0.35602362265798099</v>
+        <v>-0.356023622657981</v>
       </c>
       <c r="G35" s="1">
         <v>16380672</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
       <c r="A36" s="1">
         <v>1994</v>
       </c>
-      <c r="B36" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>38</v>
+      <c r="B36" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="D36" s="1">
-        <v>64.900000000000006</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>39</v>
+        <v>64.9</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="F36" s="1">
         <v>-1.44442551102409</v>
@@ -1508,44 +1504,44 @@
         <v>16145766</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
       <c r="A37" s="1">
         <v>1995</v>
       </c>
-      <c r="B37" t="s">
-        <v>34</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>40</v>
+      <c r="B37" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>44</v>
       </c>
       <c r="D37" s="1">
         <v>63.5</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>41</v>
+      <c r="E37" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="F37" s="1">
-        <v>-2.0620398175727801</v>
+        <v>-2.06203981757278</v>
       </c>
       <c r="G37" s="1">
         <v>15816243</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
       <c r="A38" s="1">
         <v>1996</v>
       </c>
-      <c r="B38" t="s">
-        <v>34</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>42</v>
+      <c r="B38" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="D38" s="1">
         <v>63.6</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>43</v>
+      <c r="E38" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="F38" s="1">
         <v>-1.51632157147922</v>
@@ -1554,159 +1550,159 @@
         <v>15578227</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
       <c r="A39" s="1">
         <v>1997</v>
       </c>
-      <c r="B39" t="s">
-        <v>34</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>44</v>
+      <c r="B39" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="D39" s="1">
         <v>64</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>45</v>
+      <c r="E39" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="F39" s="1">
-        <v>-1.5775237540609801</v>
+        <v>-1.57752375406098</v>
       </c>
       <c r="G39" s="1">
         <v>15334405</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
       <c r="A40" s="1">
         <v>1998</v>
       </c>
-      <c r="B40" t="s">
-        <v>34</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>46</v>
+      <c r="B40" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="D40" s="1">
         <v>64.5</v>
       </c>
-      <c r="E40" s="2" t="s">
-        <v>47</v>
+      <c r="E40" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="F40" s="1">
-        <v>-1.7284164484620601</v>
+        <v>-1.72841644846206</v>
       </c>
       <c r="G40" s="1">
         <v>1507164</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
       <c r="A41" s="1">
         <v>1999</v>
       </c>
-      <c r="B41" t="s">
-        <v>34</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>46</v>
+      <c r="B41" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="D41" s="1">
         <v>65.63</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>48</v>
+      <c r="E41" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="F41" s="1">
-        <v>-0.95511348167091403</v>
+        <v>-0.955113481670914</v>
       </c>
       <c r="G41" s="1">
         <v>14928374</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
       <c r="A42" s="1">
         <v>2000</v>
       </c>
-      <c r="B42" t="s">
-        <v>34</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>46</v>
+      <c r="B42" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="D42" s="1">
         <v>65.45</v>
       </c>
-      <c r="E42" s="2" t="s">
-        <v>49</v>
+      <c r="E42" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="F42" s="1">
-        <v>-0.30020148669052599</v>
+        <v>-0.300201486690526</v>
       </c>
       <c r="G42" s="1">
         <v>14883626</v>
       </c>
     </row>
-    <row r="43" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="19.5">
       <c r="A43" s="1">
         <v>2001</v>
       </c>
-      <c r="B43" t="s">
-        <v>34</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>50</v>
+      <c r="B43" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D43" s="1">
-        <v>65.760000000000005</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>51</v>
+        <v>65.76</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>55</v>
       </c>
       <c r="F43" s="1">
-        <v>-0.17006952632276301</v>
+        <v>-0.170069526322763</v>
       </c>
       <c r="G43" s="1">
         <v>14858335</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="19.5">
       <c r="A44" s="1">
         <v>2002</v>
       </c>
-      <c r="B44" t="s">
-        <v>34</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>44</v>
+      <c r="B44" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="D44" s="1">
         <v>65.95</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>52</v>
+      <c r="E44" s="3" t="s">
+        <v>56</v>
       </c>
       <c r="F44" s="1">
-        <v>4.1255453945045701E-3</v>
+        <v>0.00412554539450457</v>
       </c>
       <c r="G44" s="1">
         <v>14858948</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="19.5">
       <c r="A45" s="1">
         <v>2003</v>
       </c>
-      <c r="B45" t="s">
-        <v>34</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>53</v>
+      <c r="B45" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="D45" s="1">
-        <v>65.739999999999995</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>54</v>
+        <v>65.74</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>58</v>
       </c>
       <c r="F45" s="1">
         <v>0.336408913793247</v>
@@ -1715,67 +1711,67 @@
         <v>14909019</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="19.5">
       <c r="A46" s="1">
         <v>2004</v>
       </c>
-      <c r="B46" t="s">
-        <v>34</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>55</v>
+      <c r="B46" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>59</v>
       </c>
       <c r="D46" s="1">
         <v>66.06</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>56</v>
+      <c r="E46" s="3" t="s">
+        <v>60</v>
       </c>
       <c r="F46" s="1">
-        <v>0.69490948431125699</v>
+        <v>0.694909484311257</v>
       </c>
       <c r="G46" s="1">
         <v>15012984</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="19.5">
       <c r="A47" s="1">
         <v>2005</v>
       </c>
-      <c r="B47" t="s">
-        <v>34</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>57</v>
+      <c r="B47" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>61</v>
       </c>
       <c r="D47" s="1">
         <v>65.86</v>
       </c>
-      <c r="E47" s="2" t="s">
-        <v>58</v>
+      <c r="E47" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="F47" s="1">
-        <v>0.88889804270202499</v>
+        <v>0.888898042702025</v>
       </c>
       <c r="G47" s="1">
         <v>15147029</v>
       </c>
     </row>
-    <row r="48" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="19.5">
       <c r="A48" s="1">
         <v>2006</v>
       </c>
-      <c r="B48" t="s">
-        <v>34</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>59</v>
+      <c r="B48" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>63</v>
       </c>
       <c r="D48" s="1">
-        <v>66.150000000000006</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>60</v>
+        <v>66.15</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="F48" s="1">
         <v>1.05767130866502</v>
@@ -1784,67 +1780,67 @@
         <v>15308085</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="19.5">
       <c r="A49" s="1">
         <v>2007</v>
       </c>
-      <c r="B49" t="s">
-        <v>34</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>61</v>
+      <c r="B49" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>65</v>
       </c>
       <c r="D49" s="1">
         <v>66.34</v>
       </c>
-      <c r="E49" s="2" t="s">
-        <v>62</v>
+      <c r="E49" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="F49" s="1">
-        <v>1.1438512334943101</v>
+        <v>1.14385123349431</v>
       </c>
       <c r="G49" s="1">
         <v>15484192</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="19.5">
       <c r="A50" s="1">
         <v>2008</v>
       </c>
-      <c r="B50" t="s">
-        <v>34</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>63</v>
+      <c r="B50" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="D50" s="1">
         <v>67.11</v>
       </c>
-      <c r="E50" s="2" t="s">
-        <v>64</v>
+      <c r="E50" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="F50" s="1">
-        <v>1.8729620961218201</v>
+        <v>1.87296209612182</v>
       </c>
       <c r="G50" s="1">
         <v>15776938</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="19.5">
       <c r="A51" s="1">
         <v>2009</v>
       </c>
-      <c r="B51" t="s">
-        <v>34</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>65</v>
+      <c r="B51" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="D51" s="1">
         <v>68.39</v>
       </c>
-      <c r="E51" s="2" t="s">
-        <v>66</v>
+      <c r="E51" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="F51" s="1">
         <v>1.98240805691531</v>
@@ -1853,21 +1849,21 @@
         <v>16092822</v>
       </c>
     </row>
-    <row r="52" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="19.5">
       <c r="A52" s="1">
         <v>2010</v>
       </c>
-      <c r="B52" t="s">
-        <v>34</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>67</v>
+      <c r="B52" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="D52" s="1">
         <v>68.45</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>68</v>
+      <c r="E52" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="F52" s="1">
         <v>1.41327147745347</v>
@@ -1876,21 +1872,21 @@
         <v>16321872</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="19.5">
       <c r="A53" s="1">
         <v>2011</v>
       </c>
-      <c r="B53" t="s">
-        <v>34</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>67</v>
+      <c r="B53" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="D53" s="1">
         <v>68.69</v>
       </c>
-      <c r="E53" s="2" t="s">
-        <v>69</v>
+      <c r="E53" s="3" t="s">
+        <v>73</v>
       </c>
       <c r="F53" s="1">
         <v>1.43151244887822</v>
@@ -1899,21 +1895,21 @@
         <v>16557202</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="19.5">
       <c r="A54" s="1">
         <v>2012</v>
       </c>
-      <c r="B54" t="s">
-        <v>34</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>70</v>
+      <c r="B54" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="D54" s="1">
         <v>69.52</v>
       </c>
-      <c r="E54" s="2" t="s">
-        <v>71</v>
+      <c r="E54" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="F54" s="1">
         <v>1.40867688701824</v>
@@ -1922,44 +1918,44 @@
         <v>1679209</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="19.5">
       <c r="A55" s="1">
         <v>2013</v>
       </c>
-      <c r="B55" t="s">
-        <v>34</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>72</v>
+      <c r="B55" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="D55" s="1">
         <v>70.62</v>
       </c>
-      <c r="E55" s="2" t="s">
-        <v>73</v>
+      <c r="E55" s="3" t="s">
+        <v>77</v>
       </c>
       <c r="F55" s="1">
-        <v>1.4394453562479801</v>
+        <v>1.43944535624798</v>
       </c>
       <c r="G55" s="1">
         <v>17035551</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="19.5">
       <c r="A56" s="1">
         <v>2014</v>
       </c>
-      <c r="B56" t="s">
-        <v>34</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>74</v>
+      <c r="B56" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="D56" s="1">
         <v>71.44</v>
       </c>
-      <c r="E56" s="2" t="s">
-        <v>75</v>
+      <c r="E56" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="F56" s="1">
         <v>1.47267087305755</v>
@@ -1968,67 +1964,67 @@
         <v>17288285</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="19.5">
       <c r="A57" s="1">
         <v>2015</v>
       </c>
-      <c r="B57" t="s">
-        <v>34</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>76</v>
+      <c r="B57" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="D57" s="1">
         <v>71.97</v>
       </c>
-      <c r="E57" s="2" t="s">
-        <v>77</v>
+      <c r="E57" s="3" t="s">
+        <v>81</v>
       </c>
       <c r="F57" s="1">
-        <v>1.4614846851916099</v>
+        <v>1.46148468519161</v>
       </c>
       <c r="G57" s="1">
         <v>17542806</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="19.5">
       <c r="A58" s="1">
         <v>2016</v>
       </c>
-      <c r="B58" t="s">
-        <v>34</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>78</v>
+      <c r="B58" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="D58" s="1">
         <v>72.41</v>
       </c>
-      <c r="E58" s="2" t="s">
-        <v>79</v>
+      <c r="E58" s="3" t="s">
+        <v>83</v>
       </c>
       <c r="F58" s="1">
-        <v>1.4220461403292499</v>
+        <v>1.42204614032925</v>
       </c>
       <c r="G58" s="1">
         <v>17794055</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
       <c r="A59" s="1">
         <v>2017</v>
       </c>
-      <c r="B59" t="s">
-        <v>34</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>80</v>
+      <c r="B59" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>84</v>
       </c>
       <c r="D59" s="1">
         <v>72.95</v>
       </c>
-      <c r="E59" s="2" t="s">
-        <v>81</v>
+      <c r="E59" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="F59" s="1">
         <v>1.36038126908993</v>
@@ -2037,21 +2033,21 @@
         <v>18037776</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
       <c r="A60" s="1">
         <v>2018</v>
       </c>
-      <c r="B60" t="s">
-        <v>34</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>82</v>
+      <c r="B60" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>86</v>
       </c>
       <c r="D60" s="1">
-        <v>73.150000000000006</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>83</v>
+        <v>73.15</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="F60" s="1">
         <v>1.31452298457883</v>
@@ -2060,44 +2056,44 @@
         <v>18276452</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
       <c r="A61" s="1">
         <v>2019</v>
       </c>
-      <c r="B61" t="s">
-        <v>34</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>24</v>
+      <c r="B61" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="D61" s="1">
-        <v>73.180000000000007</v>
-      </c>
-      <c r="E61" s="2" t="s">
-        <v>84</v>
+        <v>73.18</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="F61" s="1">
-        <v>1.2896084895422599</v>
+        <v>1.28960848954226</v>
       </c>
       <c r="G61" s="1">
         <v>18513673</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
       <c r="A62" s="1">
         <v>2020</v>
       </c>
-      <c r="B62" t="s">
-        <v>34</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>31</v>
+      <c r="B62" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="D62" s="1">
         <v>71.37</v>
       </c>
-      <c r="E62" s="2" t="s">
-        <v>85</v>
+      <c r="E62" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="F62" s="1">
         <v>1.29863532544565</v>
@@ -2106,24 +2102,24 @@
         <v>18755666</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
       <c r="A63" s="1">
         <v>2021</v>
       </c>
-      <c r="B63" t="s">
-        <v>34</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>86</v>
+      <c r="B63" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>90</v>
       </c>
       <c r="D63" s="1">
         <v>70.23</v>
       </c>
-      <c r="E63" s="2" t="s">
-        <v>87</v>
+      <c r="E63" s="3" t="s">
+        <v>91</v>
       </c>
       <c r="F63" s="1">
-        <v>1.2995084380595501</v>
+        <v>1.29950843805955</v>
       </c>
       <c r="G63" s="1">
         <v>19000988</v>

</xml_diff>